<commit_message>
Versión 0.2 - Sección Información general
Se modificó la sección información general de acuerdo a las especificaciones acordadas
</commit_message>
<xml_diff>
--- a/BaseDeDatos/Normalización_BD.xlsx
+++ b/BaseDeDatos/Normalización_BD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/SIMOS/BD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/SIMOS/WebPage/BaseDeDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{B73878F8-670B-41D1-8CDE-8756F6565A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C529DD90-2D3D-4D91-8960-15A91105114E}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="8_{B73878F8-670B-41D1-8CDE-8756F6565A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{100CA0FC-49A1-4339-BC7F-EBA9757925EB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{C500EFD4-5021-404F-9074-B7A4C0559056}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
   <si>
     <t>Usuario</t>
   </si>
@@ -286,13 +286,19 @@
   </si>
   <si>
     <t>Documentos del proyecto</t>
+  </si>
+  <si>
+    <t>Ejercicio fiscal</t>
+  </si>
+  <si>
+    <t>ValidacionInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +330,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -345,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -358,6 +371,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,9 +1160,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0AB54B-1E2E-4E2A-8959-4106421E30E1}">
-  <dimension ref="B2:V29"/>
+  <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1277,7 +1293,7 @@
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
@@ -1294,7 +1310,7 @@
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
@@ -1308,7 +1324,7 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
         <v>67</v>
@@ -1316,7 +1332,7 @@
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
         <v>68</v>
@@ -1324,7 +1340,7 @@
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
         <v>69</v>
@@ -1332,7 +1348,7 @@
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
         <v>70</v>
@@ -1340,16 +1356,13 @@
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
       <c r="F15" t="s">
         <v>72</v>
       </c>
@@ -1402,7 +1415,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>23</v>
@@ -1443,6 +1456,11 @@
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versión 0.2 - Posicionamiento
Se agregó la posibilidad de modificar la sección opinión general
</commit_message>
<xml_diff>
--- a/BaseDeDatos/Normalización_BD.xlsx
+++ b/BaseDeDatos/Normalización_BD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/SIMOS/WebPage/BaseDeDatos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/SIMOS/SIMOS/BaseDeDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{B73878F8-670B-41D1-8CDE-8756F6565A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{100CA0FC-49A1-4339-BC7F-EBA9757925EB}"/>
+  <xr:revisionPtr revIDLastSave="445" documentId="8_{B73878F8-670B-41D1-8CDE-8756F6565A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62FD0AE4-D273-4D02-84EC-A9A5B4E5627D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{C500EFD4-5021-404F-9074-B7A4C0559056}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{C500EFD4-5021-404F-9074-B7A4C0559056}"/>
   </bookViews>
   <sheets>
     <sheet name="Definición de tablas" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
   <si>
     <t>Usuario</t>
   </si>
@@ -276,29 +276,107 @@
     <t>ID_OpinionGeneral</t>
   </si>
   <si>
-    <t>ID_FichaTecnicaProyecto</t>
-  </si>
-  <si>
-    <t>ID_FichaTecnicaEvaluacion</t>
-  </si>
-  <si>
-    <t>ID_DocumentosProyecto</t>
-  </si>
-  <si>
-    <t>Documentos del proyecto</t>
-  </si>
-  <si>
-    <t>Ejercicio fiscal</t>
-  </si>
-  <si>
-    <t>ValidacionInfo</t>
+    <t>EjercicioFiscal</t>
+  </si>
+  <si>
+    <t>InstanciaEvaluadora</t>
+  </si>
+  <si>
+    <t>Nombre DeLaEvaluacion</t>
+  </si>
+  <si>
+    <t>TipoDeEvaluacion</t>
+  </si>
+  <si>
+    <t>AñoDeEvaluacion</t>
+  </si>
+  <si>
+    <t>NombreDelInforme</t>
+  </si>
+  <si>
+    <t>URL_Informe</t>
+  </si>
+  <si>
+    <t>CostoEvaluacion</t>
+  </si>
+  <si>
+    <t>OpinionGeneral</t>
+  </si>
+  <si>
+    <t>ComentariosGenerales</t>
+  </si>
+  <si>
+    <t>ID_Observacion</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>ConObservacion</t>
+  </si>
+  <si>
+    <t>IconoEstado</t>
+  </si>
+  <si>
+    <t>ID_ComentarioObservacionEspecificoPorTema</t>
+  </si>
+  <si>
+    <t>Titulo</t>
+  </si>
+  <si>
+    <t>ID_Tema</t>
+  </si>
+  <si>
+    <t>ComentariosYObservacionesEspecificosPorTema</t>
+  </si>
+  <si>
+    <t>Tema</t>
+  </si>
+  <si>
+    <t>ContenidoDelTema</t>
+  </si>
+  <si>
+    <t>TituloDelTema</t>
+  </si>
+  <si>
+    <t>ProgramaProyecto</t>
+  </si>
+  <si>
+    <t>ID_ProgramaProyecto</t>
+  </si>
+  <si>
+    <t>Clave</t>
+  </si>
+  <si>
+    <t>Etapa</t>
+  </si>
+  <si>
+    <t>SubEtapa</t>
+  </si>
+  <si>
+    <t>EstadoValidacion</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t>ID_Evaluacion</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>Sección</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,13 +408,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -358,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,7 +442,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0AB54B-1E2E-4E2A-8959-4106421E30E1}">
-  <dimension ref="B2:V30"/>
+  <dimension ref="B2:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,17 +1241,19 @@
     <col min="1" max="1" width="3.77734375" customWidth="1"/>
     <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.77734375" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" customWidth="1"/>
     <col min="5" max="5" width="3.77734375" customWidth="1"/>
-    <col min="6" max="6" width="44.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.77734375" customWidth="1"/>
-    <col min="8" max="8" width="30.21875" customWidth="1"/>
+    <col min="8" max="8" width="46.88671875" customWidth="1"/>
     <col min="9" max="9" width="3.77734375" customWidth="1"/>
-    <col min="10" max="10" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.77734375" customWidth="1"/>
+    <col min="12" max="12" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="4">
         <v>1</v>
       </c>
@@ -1191,39 +1263,32 @@
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="4">
-        <v>7</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="2:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>107</v>
+      </c>
       <c r="H3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1237,230 +1302,202 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>49</v>
       </c>
       <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="F13" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="H18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="F16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="6" t="s">
-        <v>84</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="H24" s="4">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.4 - Creación de la vista para el usuario administrador
Se creó la vista para el usuario administrador solo en el front-end
</commit_message>
<xml_diff>
--- a/BaseDeDatos/Normalización_BD.xlsx
+++ b/BaseDeDatos/Normalización_BD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seggtogob-my.sharepoint.com/personal/wa_moreno_seg_guanajuato_gob_mx/Documents/Proyectos/Proyectos_de_software/SIMOS/SIMOS/BaseDeDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="445" documentId="8_{B73878F8-670B-41D1-8CDE-8756F6565A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62FD0AE4-D273-4D02-84EC-A9A5B4E5627D}"/>
+  <xr:revisionPtr revIDLastSave="597" documentId="8_{B73878F8-670B-41D1-8CDE-8756F6565A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B470E2E9-C097-45D4-81F1-1CB5BA60D073}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="2" xr2:uid="{C500EFD4-5021-404F-9074-B7A4C0559056}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Definición de tablas" sheetId="1" r:id="rId1"/>
     <sheet name="1ra Forma Normal" sheetId="3" r:id="rId2"/>
     <sheet name="2da Forma Nomal" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="119">
   <si>
     <t>Usuario</t>
   </si>
@@ -370,6 +371,30 @@
   </si>
   <si>
     <t>Sección</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>NombreResponsable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>INT,</t>
+  </si>
+  <si>
+    <t>DependenciaResponsable</t>
+  </si>
+  <si>
+    <t>UnidadReponsable</t>
+  </si>
+  <si>
+    <t>SiglasUR</t>
+  </si>
+  <si>
+    <t>EstadioValidación</t>
   </si>
 </sst>
 </file>
@@ -417,7 +442,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -425,11 +450,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -442,6 +482,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,6 +506,400 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>173429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>137161</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312EAC32-4B8F-2CD8-242F-A8AB9C824A65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="83917" b="72934"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304800" y="173429"/>
+          <a:ext cx="1828800" cy="1243892"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>158188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>746760</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A466A498-064E-4A33-9FA2-575E9A722B00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="16686" r="67231" b="42923"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2087880" y="158188"/>
+          <a:ext cx="1828800" cy="2623111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE0583B9-8069-4E8C-AF98-F1DEF09AA6BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="332" t="50240" r="83919" b="14941"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="327660" y="1524000"/>
+          <a:ext cx="1790700" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3BF7859-909D-4BFC-B2A3-33BC9EA329F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="33372" t="167" r="48601" b="57221"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3947160" y="182880"/>
+          <a:ext cx="2049780" cy="1958340"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7319A16-CD4F-47B4-AC24-BEF390858577}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="51869" t="330" r="22130" b="68332"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5966460" y="2423160"/>
+          <a:ext cx="2956560" cy="1440180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BCC34D-6DC9-4C73-BE14-9D824C30B673}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="78270" t="-829" r="-49" b="50590"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5951220" y="121920"/>
+          <a:ext cx="2476500" cy="2308860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4477C808-E79D-45A5-8026-4BADBB3145A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="51600" t="49907" r="22198" b="31854"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2080260" y="2781300"/>
+          <a:ext cx="2979420" cy="838200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>45721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>74335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagen 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26BA2B4F-23CA-4A9C-1740-6552CF9B76D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2118360" y="3520441"/>
+          <a:ext cx="2887980" cy="943014"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>45721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>392944</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>175261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249013A5-56C1-CACB-2D68-20D50DCE6852}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5082540" y="3886201"/>
+          <a:ext cx="2442724" cy="861060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -988,7 +1431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D653D5F-8629-425A-82BC-BBFFACA01138}">
   <dimension ref="B2:V23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1230,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0AB54B-1E2E-4E2A-8959-4106421E30E1}">
-  <dimension ref="B2:X30"/>
+  <dimension ref="B1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1247,12 +1692,13 @@
     <col min="7" max="7" width="3.77734375" customWidth="1"/>
     <col min="8" max="8" width="46.88671875" customWidth="1"/>
     <col min="9" max="9" width="3.77734375" customWidth="1"/>
-    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.77734375" customWidth="1"/>
     <col min="12" max="12" width="42.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:24" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:24" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="4">
         <v>1</v>
@@ -1267,31 +1713,41 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="4">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="J2" s="6">
+        <v>8</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="L2" s="4"/>
+      <c r="L2" s="4">
+        <v>9</v>
+      </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="2:24" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="J3" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="L3" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -1306,197 +1762,292 @@
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="J4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="8" t="s">
         <v>78</v>
       </c>
+      <c r="J5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>11</v>
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" t="s">
-        <v>110</v>
-      </c>
-      <c r="L8" s="3"/>
+      <c r="D8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D12" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="J13" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
+      <c r="J14" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="F13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
-        <v>106</v>
+      <c r="J15" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:24" ht="18" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="4">
+        <v>6</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24" s="4">
         <v>5</v>
       </c>
-      <c r="H16" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="H18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" t="s">
+    </row>
+    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H26" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="H24" s="4">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H25" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H27" t="s">
-        <v>89</v>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H28" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H30" t="s">
+      <c r="H29" s="8" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1504,4 +2055,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF7AD7F-D8F7-443F-AD5D-D955DC8AA6B6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>